<commit_message>
Ajustes após testes finais
</commit_message>
<xml_diff>
--- a/Data/Output/Report.xlsx
+++ b/Data/Output/Report.xlsx
@@ -85,13 +85,13 @@
     <x:t>246318 USD</x:t>
   </x:si>
   <x:si>
-    <x:t>5.4466</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32.6796</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 22:59:36</x:t>
+    <x:t>229145.53009999997</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1374873.1805999998</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-07-09 21:28:45</x:t>
   </x:si>
   <x:si>
     <x:t>Rua Antônio de Godói</x:t>
@@ -127,13 +127,13 @@
     <x:t>204472 EUR</x:t>
   </x:si>
   <x:si>
-    <x:t>6.38162</x:t>
-  </x:si>
-  <x:si>
-    <x:t>51.05296</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 21:55:11</x:t>
+    <x:t>167380.52361</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1339044.18888</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-07-09 21:05:57</x:t>
   </x:si>
   <x:si>
     <x:t>Avenida São João</x:t>
@@ -163,13 +163,13 @@
     <x:t>133375 RON</x:t>
   </x:si>
   <x:si>
-    <x:t>1.25657227</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6.282861349999999</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 22:08:52</x:t>
+    <x:t>34426.8515635</x:t>
+  </x:si>
+  <x:si>
+    <x:t>172134.25781749998</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-07-09 21:41:03</x:t>
   </x:si>
   <x:si>
     <x:t>Avenida Senador Queirós</x:t>
@@ -199,13 +199,10 @@
     <x:t>203623 USD</x:t>
   </x:si>
   <x:si>
-    <x:t>5.4465</x:t>
-  </x:si>
-  <x:si>
-    <x:t>38.1255</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 22:49:34</x:t>
+    <x:t>162366.07129999998</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1136562.4991</x:t>
   </x:si>
   <x:si>
     <x:t>Rua Augusto Severo</x:t>
@@ -232,6 +229,15 @@
     <x:t>5155 RON</x:t>
   </x:si>
   <x:si>
+    <x:t>1330.6123322199999</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6653.0616611</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rua Líbero Badaró</x:t>
+  </x:si>
+  <x:si>
     <x:t>O Vendor ID informado não está no formato válido</x:t>
   </x:si>
   <x:si>
@@ -253,13 +259,10 @@
     <x:t>88032 EUR</x:t>
   </x:si>
   <x:si>
-    <x:t>6.37755</x:t>
-  </x:si>
-  <x:si>
-    <x:t>51.0204</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 22:39:31</x:t>
+    <x:t>72062.88516</x:t>
+  </x:si>
+  <x:si>
+    <x:t>576503.08128</x:t>
   </x:si>
   <x:si>
     <x:t>Rua Boa Vista</x:t>
@@ -283,6 +286,12 @@
     <x:t>83007 RON</x:t>
   </x:si>
   <x:si>
+    <x:t>11903.23718726</x:t>
+  </x:si>
+  <x:si>
+    <x:t>107129.13468534</x:t>
+  </x:si>
+  <x:si>
     <x:t>A data da invoice está em um formato inválido ou fora do intervalo permitido: entre os anos de 2018 e 2021.</x:t>
   </x:si>
   <x:si>
@@ -301,6 +310,12 @@
     <x:t>101118 EUR</x:t>
   </x:si>
   <x:si>
+    <x:t>220733.51574</x:t>
+  </x:si>
+  <x:si>
+    <x:t>662200.5472200001</x:t>
+  </x:si>
+  <x:si>
     <x:t>982763</x:t>
   </x:si>
   <x:si>
@@ -313,10 +328,10 @@
     <x:t>62685 EUR</x:t>
   </x:si>
   <x:si>
-    <x:t>44.67134</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 22:05:32</x:t>
+    <x:t>58644.414450000004</x:t>
+  </x:si>
+  <x:si>
+    <x:t>410510.90115000005</x:t>
   </x:si>
   <x:si>
     <x:t>231319</x:t>
@@ -331,6 +346,12 @@
     <x:t>199584 EUR</x:t>
   </x:si>
   <x:si>
+    <x:t>163379.21292000002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1307033.7033600002</x:t>
+  </x:si>
+  <x:si>
     <x:t>526408</x:t>
   </x:si>
   <x:si>
@@ -343,7 +364,10 @@
     <x:t>286085 USD</x:t>
   </x:si>
   <x:si>
-    <x:t>27.233</x:t>
+    <x:t>319368.12889999995</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1596840.6445</x:t>
   </x:si>
   <x:si>
     <x:t>147239</x:t>
@@ -358,7 +382,10 @@
     <x:t>328950 EUR</x:t>
   </x:si>
   <x:si>
-    <x:t>63.7755</x:t>
+    <x:t>215422.44705000002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2154224.4705000003</x:t>
   </x:si>
   <x:si>
     <x:t>296596</x:t>
@@ -373,7 +400,10 @@
     <x:t>19576 USD</x:t>
   </x:si>
   <x:si>
-    <x:t>43.5728</x:t>
+    <x:t>13658.419899999999</x:t>
+  </x:si>
+  <x:si>
+    <x:t>109267.35919999999</x:t>
   </x:si>
   <x:si>
     <x:t>955164</x:t>
@@ -394,6 +424,18 @@
     <x:t>358200 CAD</x:t>
   </x:si>
   <x:si>
+    <x:t>162217.636</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1459958.7240000002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-07-09 21:25:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rua São Bento</x:t>
+  </x:si>
+  <x:si>
     <x:t>349606</x:t>
   </x:si>
   <x:si>
@@ -403,6 +445,9 @@
     <x:t>332614 USD</x:t>
   </x:si>
   <x:si>
+    <x:t>1856551.5638</x:t>
+  </x:si>
+  <x:si>
     <x:t>680422</x:t>
   </x:si>
   <x:si>
@@ -415,6 +460,12 @@
     <x:t>186975 USD</x:t>
   </x:si>
   <x:si>
+    <x:t>115959.81749999999</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1043638.3574999999</x:t>
+  </x:si>
+  <x:si>
     <x:t>696770</x:t>
   </x:si>
   <x:si>
@@ -427,6 +478,12 @@
     <x:t>298040 EUR</x:t>
   </x:si>
   <x:si>
+    <x:t>243975.17145000002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1951801.3716000002</x:t>
+  </x:si>
+  <x:si>
     <x:t>101435</x:t>
   </x:si>
   <x:si>
@@ -448,6 +505,15 @@
     <x:t>48072 RON</x:t>
   </x:si>
   <x:si>
+    <x:t>31020.94861032</x:t>
+  </x:si>
+  <x:si>
+    <x:t>62041.89722064</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ladeira da Memória</x:t>
+  </x:si>
+  <x:si>
     <x:t>362980</x:t>
   </x:si>
   <x:si>
@@ -466,13 +532,10 @@
     <x:t>180900 RON</x:t>
   </x:si>
   <x:si>
-    <x:t>1.25659472</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12.5659472</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 23:01:19</x:t>
+    <x:t>23347.0194858</x:t>
+  </x:si>
+  <x:si>
+    <x:t>233470.194858</x:t>
   </x:si>
   <x:si>
     <x:t>Rua do Centro</x:t>
@@ -490,6 +553,12 @@
     <x:t>141872 USD</x:t>
   </x:si>
   <x:si>
+    <x:t>98985.86779999999</x:t>
+  </x:si>
+  <x:si>
+    <x:t>791886.9423999999</x:t>
+  </x:si>
+  <x:si>
     <x:t>570199</x:t>
   </x:si>
   <x:si>
@@ -508,6 +577,15 @@
     <x:t>343728 USD</x:t>
   </x:si>
   <x:si>
+    <x:t>213176.28639999998</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1918586.5776</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rua do Comércio</x:t>
+  </x:si>
+  <x:si>
     <x:t>O 'VENDOR ID' informado não foi encontrado na tabela auxiliar ou está com status diferente de 'CHECKED'.</x:t>
   </x:si>
   <x:si>
@@ -523,7 +601,10 @@
     <x:t>113412 USD</x:t>
   </x:si>
   <x:si>
-    <x:t>32.679</x:t>
+    <x:t>105505.2934</x:t>
+  </x:si>
+  <x:si>
+    <x:t>633031.7603999999</x:t>
   </x:si>
   <x:si>
     <x:t>568949</x:t>
@@ -544,6 +625,15 @@
     <x:t>284837 RON</x:t>
   </x:si>
   <x:si>
+    <x:t>52515.95190142</x:t>
+  </x:si>
+  <x:si>
+    <x:t>367611.66330993996</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rua do Tesouro</x:t>
+  </x:si>
+  <x:si>
     <x:t>867556</x:t>
   </x:si>
   <x:si>
@@ -556,6 +646,12 @@
     <x:t>77520 EUR</x:t>
   </x:si>
   <x:si>
+    <x:t>50766.22008</x:t>
+  </x:si>
+  <x:si>
+    <x:t>507662.20080000005</x:t>
+  </x:si>
+  <x:si>
     <x:t>421789</x:t>
   </x:si>
   <x:si>
@@ -586,7 +682,10 @@
     <x:t>184923 EUR</x:t>
   </x:si>
   <x:si>
-    <x:t>57.39795</x:t>
+    <x:t>134557.98813</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1211021.89317</x:t>
   </x:si>
   <x:si>
     <x:t>Rua Alexandre Mackenzie</x:t>
@@ -607,7 +706,7 @@
     <x:t>176729 EUR</x:t>
   </x:si>
   <x:si>
-    <x:t>Rua do Tesouro</x:t>
+    <x:t>1157361.10791</x:t>
   </x:si>
   <x:si>
     <x:t>951433</x:t>
@@ -619,10 +718,10 @@
     <x:t>2 BTC</x:t>
   </x:si>
   <x:si>
-    <x:t>595926</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-07-08 23:04:20</x:t>
+    <x:t>1225806</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-07-09 21:27:14</x:t>
   </x:si>
   <x:si>
     <x:t>145432</x:t>
@@ -637,7 +736,10 @@
     <x:t>175050 USD</x:t>
   </x:si>
   <x:si>
-    <x:t>49.019400000000005</x:t>
+    <x:t>108564.06499999999</x:t>
+  </x:si>
+  <x:si>
+    <x:t>977076.585</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1214,10 +1316,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
         <x:v>63</x:v>
-      </x:c>
-      <x:c r="L5" s="0" t="s">
-        <x:v>64</x:v>
       </x:c>
       <x:c r="M5" s="0" t="s">
         <x:v>27</x:v>
@@ -1231,63 +1333,63 @@
     </x:row>
     <x:row r="6" spans="1:15">
       <x:c r="A6" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="E6" s="0" t="s">
         <x:v>68</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>69</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="H6" s="0" t="s">
+      <x:c r="I6" s="0" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="L6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="M6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O6" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:15">
       <x:c r="A7" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>57</x:v>
@@ -1296,22 +1398,22 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L7" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="M7" s="0" t="s">
         <x:v>27</x:v>
@@ -1325,10 +1427,10 @@
     </x:row>
     <x:row r="8" spans="1:15">
       <x:c r="A8" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>17</x:v>
@@ -1337,45 +1439,45 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="J8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="K8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="L8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="M8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O8" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:15">
       <x:c r="A9" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>55</x:v>
@@ -1384,75 +1486,75 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="K9" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="L9" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="M9" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="N9" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="O9" s="0" t="s">
         <x:v>92</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="H9" s="0" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="I9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="J9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="K9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="L9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="M9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="N9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="O9" s="0" t="s">
-        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:15">
       <x:c r="A10" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="J10" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L10" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="M10" s="0" t="s">
         <x:v>27</x:v>
@@ -1466,10 +1568,10 @@
     </x:row>
     <x:row r="11" spans="1:15">
       <x:c r="A11" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>17</x:v>
@@ -1484,19 +1586,19 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="K11" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L11" s="0" t="s">
         <x:v>26</x:v>
@@ -1513,40 +1615,40 @@
     </x:row>
     <x:row r="12" spans="1:15">
       <x:c r="A12" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="J12" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="K12" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
       <x:c r="L12" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="M12" s="0" t="s">
         <x:v>27</x:v>
@@ -1560,7 +1662,7 @@
     </x:row>
     <x:row r="13" spans="1:15">
       <x:c r="A13" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>42</x:v>
@@ -1572,28 +1674,28 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="J13" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="K13" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L13" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="M13" s="0" t="s">
         <x:v>27</x:v>
@@ -1607,10 +1709,10 @@
     </x:row>
     <x:row r="14" spans="1:15">
       <x:c r="A14" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
         <x:v>32</x:v>
@@ -1625,16 +1727,16 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="J14" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="K14" s="0" t="s">
         <x:v>25</x:v>
@@ -1654,57 +1756,57 @@
     </x:row>
     <x:row r="15" spans="1:15">
       <x:c r="A15" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="I15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="J15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="K15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="L15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="M15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O15" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:15">
       <x:c r="A16" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
         <x:v>32</x:v>
@@ -1716,19 +1818,19 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="I16" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="J16" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="K16" s="0" t="s">
         <x:v>25</x:v>
@@ -1748,87 +1850,87 @@
     </x:row>
     <x:row r="17" spans="1:15">
       <x:c r="A17" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="J17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="K17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="M17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N17" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O17" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:15">
       <x:c r="A18" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="I18" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="J18" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="K18" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L18" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="M18" s="0" t="s">
         <x:v>27</x:v>
@@ -1842,90 +1944,90 @@
     </x:row>
     <x:row r="19" spans="1:15">
       <x:c r="A19" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="I19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="J19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="K19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="L19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="M19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N19" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O19" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:15">
       <x:c r="A20" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="I20" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="J20" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="K20" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="L20" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="M20" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="N20" s="0" t="s">
         <x:v>28</x:v>
@@ -1936,10 +2038,10 @@
     </x:row>
     <x:row r="21" spans="1:15">
       <x:c r="A21" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
         <x:v>17</x:v>
@@ -1948,22 +2050,22 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="I21" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="J21" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="K21" s="0" t="s">
         <x:v>25</x:v>
@@ -1983,87 +2085,87 @@
     </x:row>
     <x:row r="22" spans="1:15">
       <x:c r="A22" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="H22" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="I22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="J22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="K22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="M22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O22" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>190</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:15">
       <x:c r="A23" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="H23" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="I23" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="J23" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="K23" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="L23" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="M23" s="0" t="s">
         <x:v>27</x:v>
@@ -2077,16 +2179,16 @@
     </x:row>
     <x:row r="24" spans="1:15">
       <x:c r="A24" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
         <x:v>19</x:v>
@@ -2095,39 +2197,39 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="H24" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="I24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="J24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="K24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="L24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="M24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N24" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O24" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:15">
       <x:c r="A25" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
         <x:v>32</x:v>
@@ -2139,22 +2241,22 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="H25" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="I25" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="J25" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="K25" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L25" s="0" t="s">
         <x:v>40</x:v>
@@ -2171,28 +2273,28 @@
     </x:row>
     <x:row r="26" spans="1:15">
       <x:c r="A26" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="H26" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="I26" s="0" t="s">
         <x:v>29</x:v>
@@ -2213,51 +2315,51 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="O26" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>217</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:15">
       <x:c r="A27" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="H27" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="I27" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="J27" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="K27" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L27" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="M27" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="N27" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="O27" s="0" t="s">
         <x:v>29</x:v>
@@ -2265,40 +2367,40 @@
     </x:row>
     <x:row r="28" spans="1:15">
       <x:c r="A28" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="H28" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="I28" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="J28" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="K28" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L28" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="M28" s="0" t="s">
         <x:v>27</x:v>
@@ -2312,10 +2414,10 @@
     </x:row>
     <x:row r="29" spans="1:15">
       <x:c r="A29" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
         <x:v>17</x:v>
@@ -2324,25 +2426,25 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="H29" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="I29" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="J29" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="K29" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="L29" s="0" t="s">
         <x:v>26</x:v>
@@ -2359,10 +2461,10 @@
     </x:row>
     <x:row r="30" spans="1:15">
       <x:c r="A30" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>55</x:v>
@@ -2371,28 +2473,28 @@
         <x:v>56</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="H30" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="I30" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="J30" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="K30" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
       <x:c r="L30" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="M30" s="0" t="s">
         <x:v>27</x:v>

</xml_diff>